<commit_message>
KIBON-120: Zahlungen and Massenversand statistic translated
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4226206D-1B93-46B8-B21B-ED1B25CF4B94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12675" yWindow="4680" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="12675" yWindow="4680" windowWidth="28800" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -26,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
-    <t>Institution</t>
-  </si>
-  <si>
     <t>{institution}</t>
   </si>
   <si>
@@ -59,40 +57,9 @@
     <t>{betragCHF}</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Geb. Datum</t>
-  </si>
-  <si>
-    <t>Verfügung</t>
-  </si>
-  <si>
-    <t>Von</t>
-  </si>
-  <si>
-    <t>Bis</t>
-  </si>
-  <si>
-    <t>BG-Pensum</t>
-  </si>
-  <si>
-    <t>Betrag in CHF</t>
-  </si>
-  <si>
-    <t>In Zahlungslauf
-ignorieren</t>
-  </si>
-  <si>
     <t>{isIgnoriert}</t>
   </si>
   <si>
-    <t>Korrektur</t>
-  </si>
-  <si>
     <t>{isKorrektur}</t>
   </si>
   <si>
@@ -105,16 +72,49 @@
     <t>{faelligAm}</t>
   </si>
   <si>
-    <t>generiert am</t>
-  </si>
-  <si>
-    <t>faellig am</t>
+    <t>{generiertAmTitle}</t>
+  </si>
+  <si>
+    <t>{faelligAmTitle}</t>
+  </si>
+  <si>
+    <t>{institutionTitle}</t>
+  </si>
+  <si>
+    <t>{nachnameTitle}</t>
+  </si>
+  <si>
+    <t>{vornameTitle}</t>
+  </si>
+  <si>
+    <t>{geburtsdatumTitle}</t>
+  </si>
+  <si>
+    <t>{verfuegungTitle}</t>
+  </si>
+  <si>
+    <t>{vonTitle}</t>
+  </si>
+  <si>
+    <t>{bisTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensumTitle}</t>
+  </si>
+  <si>
+    <t>{betragCHFTitle}</t>
+  </si>
+  <si>
+    <t>{korrekturTitle}</t>
+  </si>
+  <si>
+    <t>{zahlungIgnorierenTitle}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$CHF]\ #,##0.00;[Red]\-[$CHF]\ #,##0.00"/>
@@ -213,27 +213,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -548,11 +528,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +553,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -591,91 +571,91 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" t="s">
         <v>7</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +663,7 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A7:XFD999999">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$J7="X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
KIBON-112: Zahlungslauf muss pro Gemeinde sein. Gemeindeabhängigkeit in den Services eingebaut. Reports angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\reporting_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\M$\hefr\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C65D09-DC5C-4C4C-B9DB-C6C3EC039E40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12672" yWindow="4680" windowWidth="28800" windowHeight="14016"/>
+    <workbookView xWindow="31995" yWindow="795" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>{institution}</t>
   </si>
@@ -108,12 +109,18 @@
   </si>
   <si>
     <t>{zahlungIgnorierenTitle}</t>
+  </si>
+  <si>
+    <t>{gemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{gemeinde}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$CHF]\ #,##0.00;[Red]\-[$CHF]\ #,##0.00"/>
@@ -527,30 +534,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" customWidth="1"/>
-    <col min="12" max="12" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
@@ -565,10 +572,10 @@
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -576,7 +583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -584,76 +591,84 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -661,9 +676,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:XFD999999">
+  <conditionalFormatting sqref="A8:XFD1000000">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$J7="X"</formula>
+      <formula>$J8="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
KIBON-122: Angebotstyp auf GUI und in Reports hinzugefügt
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\M$\hefr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C65D09-DC5C-4C4C-B9DB-C6C3EC039E40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAA5E19-D769-428D-9F7B-83133A216200}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31995" yWindow="795" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>{institution}</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>{gemeinde}</t>
+  </si>
+  <si>
+    <t>{betreuungsangebotTyp}</t>
+  </si>
+  <si>
+    <t>{betreuungsangebotTypTitle}</t>
   </si>
 </sst>
 </file>
@@ -535,29 +541,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
@@ -571,11 +577,13 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -583,7 +591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -591,7 +599,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -599,86 +607,92 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="K8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="L8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:XFD1000000">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$J8="X"</formula>
+      <formula>$K8="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
KIBON-1019: Rausfiltern von Korrekturen, die eigentlich keine sind (Summe = 9)
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\M$\hefr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAA5E19-D769-428D-9F7B-83133A216200}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1261BE-0888-4D5A-A065-1037E6A94FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31995" yWindow="795" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="7095" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -220,6 +220,9 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,12 +547,13 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
@@ -661,7 +665,7 @@
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="6" t="s">

</xml_diff>

<commit_message>
KIBON-1344: Report Zahlungen Totals: Template angepasst, Mergefields ergaenzt, Uebersetzungen eingefuegt
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1261BE-0888-4D5A-A065-1037E6A94FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9852D93-EEED-4460-9115-7FAC2859AA23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="7095" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Totals" sheetId="3" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>{institution}</t>
   </si>
@@ -121,6 +122,72 @@
   </si>
   <si>
     <t>{betreuungsangebotTypTitle}</t>
+  </si>
+  <si>
+    <t>{institutionIdTitle}</t>
+  </si>
+  <si>
+    <t>{institutionId}</t>
+  </si>
+  <si>
+    <t>{traegerschaftTitle}</t>
+  </si>
+  <si>
+    <t>{traegerschaft}</t>
+  </si>
+  <si>
+    <t>{betragAusbezahltTitle}</t>
+  </si>
+  <si>
+    <t>{betragAusbezahlt}</t>
+  </si>
+  <si>
+    <t>{ibanTitle}</t>
+  </si>
+  <si>
+    <t>{iban}</t>
+  </si>
+  <si>
+    <t>{kontoinhaberTitle}</t>
+  </si>
+  <si>
+    <t>{kontoinhaber}</t>
+  </si>
+  <si>
+    <t>{organisationTitle}</t>
+  </si>
+  <si>
+    <t>{organisation}</t>
+  </si>
+  <si>
+    <t>{auszahlungTitle}</t>
+  </si>
+  <si>
+    <t>{strasseTitle}</t>
+  </si>
+  <si>
+    <t>{strasse}</t>
+  </si>
+  <si>
+    <t>{hausnummerTitle}</t>
+  </si>
+  <si>
+    <t>{hausnummer}</t>
+  </si>
+  <si>
+    <t>{plzTitle}</t>
+  </si>
+  <si>
+    <t>{plz}</t>
+  </si>
+  <si>
+    <t>{ortTitle}</t>
+  </si>
+  <si>
+    <t>{ort}</t>
+  </si>
+  <si>
+    <t>{repeatZahlungTotalsRow}</t>
   </si>
 </sst>
 </file>
@@ -168,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -191,11 +258,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -218,17 +322,58 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -543,11 +688,215 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002696E7-1347-4331-86FF-AE08C25E0F9C}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E6" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A9:XFD999992 G8:K8 B8 D8:E8 N8:XFD8">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>#REF!="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>#REF!="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>#REF!="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$K8="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$K8="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M8">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$K8="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,20 +917,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -665,7 +1014,7 @@
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -695,7 +1044,7 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:XFD1000000">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$K8="X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
KIBON-1512: Excel-Template angepasst fuer Mahlzeiten-Zahlungslaeufe: Es braucht eine zusaetzliche Spalte fuer den Antragsteller
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\kiBon\statistiken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9852D93-EEED-4460-9115-7FAC2859AA23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BD19EB-865E-4EC6-B2FA-FCBD208E39DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2700" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>{institution}</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>{repeatZahlungTotalsRow}</t>
+  </si>
+  <si>
+    <t>{antragstellerTitle}</t>
+  </si>
+  <si>
+    <t>{antragsteller}</t>
+  </si>
+  <si>
+    <t>{repeatAntragsteller}</t>
   </si>
 </sst>
 </file>
@@ -327,9 +336,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -338,6 +344,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,46 +698,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002696E7-1347-4331-86FF-AE08C25E0F9C}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="3" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-    </row>
-    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -736,7 +745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -744,7 +753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -752,19 +761,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="16" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -778,31 +790,34 @@
         <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -815,76 +830,79 @@
       <c r="D8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="K8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="L8" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="M8" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D11" s="14"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E6:L6"/>
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="F6:M6"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:XFD999992 G8:K8 B8 D8:E8 N8:XFD8">
-    <cfRule type="expression" dxfId="5" priority="6">
+  <conditionalFormatting sqref="A9:XFD999992 H8:L8 B8 O8:XFD8 F8 D8">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>#REF!="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <conditionalFormatting sqref="M8">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>#REF!="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="G8">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>#REF!="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$K8="X"</formula>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$L8="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$K8="X"</formula>
+  <conditionalFormatting sqref="C8:D8">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$L8="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$K8="X"</formula>
+  <conditionalFormatting sqref="N8">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$L8="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -917,20 +935,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -1044,7 +1062,7 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:XFD1000000">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$K8="X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
KIBON-1771 Add second antragsteller to Mahlzeiten Zahlung file
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\kiBon\statistiken\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BD19EB-865E-4EC6-B2FA-FCBD208E39DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D565B032-53C1-4479-88D6-E624BCF0B86C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2700" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>{institution}</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>{repeatAntragsteller}</t>
+  </si>
+  <si>
+    <t>{repeatAntragsteller2}</t>
+  </si>
+  <si>
+    <t>{antragsteller2Title}</t>
+  </si>
+  <si>
+    <t>{antragsteller2}</t>
   </si>
 </sst>
 </file>
@@ -352,7 +361,12 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -698,25 +712,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002696E7-1347-4331-86FF-AE08C25E0F9C}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="3" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>12</v>
       </c>
@@ -732,12 +746,13 @@
       <c r="K1" s="18"/>
       <c r="L1" s="18"/>
       <c r="M1" s="18"/>
-    </row>
-    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="N1" s="18"/>
+    </row>
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -745,7 +760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -753,7 +768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -761,22 +776,25 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="16"/>
+      <c r="N6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -793,31 +811,34 @@
         <v>54</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -833,35 +854,38 @@
       <c r="E8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="K8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="L8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="M8" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="N8" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -869,40 +893,46 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F6:M6"/>
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="G6:N6"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:XFD999992 H8:L8 B8 O8:XFD8 F8 D8">
+  <conditionalFormatting sqref="A9:E999992 I8:M8 B8 P8:XFD8 G8 D8 G9:XFD999992">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>#REF!="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8">
     <cfRule type="expression" dxfId="6" priority="6">
       <formula>#REF!="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
+  <conditionalFormatting sqref="H8">
     <cfRule type="expression" dxfId="5" priority="5">
       <formula>#REF!="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
+  <conditionalFormatting sqref="A8">
     <cfRule type="expression" dxfId="4" priority="4">
-      <formula>#REF!="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>$L8="X"</formula>
+      <formula>$M8="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:D8">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$L8="X"</formula>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$M8="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$L8="X"</formula>
+  <conditionalFormatting sqref="O8">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$M8="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:F999992">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>#REF!="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1062,7 +1092,7 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:XFD1000000">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$K8="X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
KIBON-1771 hide columns manually since RepeatCol didn't work correctly
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D565B032-53C1-4479-88D6-E624BCF0B86C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169EE4C8-B325-47C0-A0B1-52A18322B93E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>{institution}</t>
   </si>
@@ -194,12 +194,6 @@
   </si>
   <si>
     <t>{antragsteller}</t>
-  </si>
-  <si>
-    <t>{repeatAntragsteller}</t>
-  </si>
-  <si>
-    <t>{repeatAntragsteller2}</t>
   </si>
   <si>
     <t>{antragsteller2Title}</t>
@@ -317,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -345,6 +339,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,12 +356,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -714,9 +704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002696E7-1347-4331-86FF-AE08C25E0F9C}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -731,22 +719,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -777,22 +765,16 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -811,7 +793,7 @@
         <v>54</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>36</v>
@@ -855,7 +837,7 @@
         <v>55</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>37</v>
@@ -896,17 +878,11 @@
       <c r="L11" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="G6:N6"/>
-    <mergeCell ref="A1:N1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:E999992 I8:M8 B8 P8:XFD8 G8 D8 G9:XFD999992">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>#REF!="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N8">
-    <cfRule type="expression" dxfId="6" priority="6">
+  <conditionalFormatting sqref="B8 P8:XFD8 D8:G8 A9:D999992 G9:XFD999992 I8:N8 E8:F999992">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>#REF!="X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -920,7 +896,7 @@
       <formula>$M8="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:D8">
+  <conditionalFormatting sqref="C8:F8">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>$M8="X"</formula>
     </cfRule>
@@ -931,7 +907,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F999992">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>#REF!="X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -965,20 +941,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -1092,7 +1068,7 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:XFD1000000">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$K8="X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>